<commit_message>
Added packages through to the year ending February 2024
</commit_message>
<xml_diff>
--- a/GB Accounts 2022-23/GB Accounts Company 2023-11-30 (Nov23) Excel 2007/CT600OnlineLookALike.xlsx
+++ b/GB Accounts 2022-23/GB Accounts Company 2023-11-30 (Nov23) Excel 2007/CT600OnlineLookALike.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64286BCF-ABB7-4EF1-93AC-F18D5E03E961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A54A47E-8884-4EE5-8764-4BB540DDE959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5885,10 +5885,10 @@
         </row>
         <row r="33">
           <cell r="A33">
-            <v>365</v>
+            <v>121</v>
           </cell>
           <cell r="C33">
-            <v>44652</v>
+            <v>44896</v>
           </cell>
           <cell r="E33">
             <v>2022</v>
@@ -5899,10 +5899,10 @@
         </row>
         <row r="34">
           <cell r="A34">
-            <v>0</v>
+            <v>244</v>
           </cell>
           <cell r="D34">
-            <v>45016</v>
+            <v>45260</v>
           </cell>
           <cell r="E34">
             <v>2023</v>
@@ -6319,7 +6319,7 @@
   <dimension ref="A1:IV2360"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6374,7 +6374,7 @@
       <c r="I2" s="283"/>
       <c r="J2" s="400">
         <f>H46</f>
-        <v>44652</v>
+        <v>44896</v>
       </c>
       <c r="K2" s="400"/>
       <c r="L2" s="400"/>
@@ -6383,7 +6383,7 @@
       </c>
       <c r="N2" s="397">
         <f>IF(H59&gt;0,H59,H51)</f>
-        <v>45016</v>
+        <v>45260</v>
       </c>
       <c r="O2" s="397"/>
       <c r="P2" s="345"/>
@@ -7249,7 +7249,7 @@
       <c r="G46" s="43"/>
       <c r="H46" s="308">
         <f>[1]CorporationTax!$C$33</f>
-        <v>44652</v>
+        <v>44896</v>
       </c>
       <c r="I46" s="309"/>
       <c r="J46" s="411"/>
@@ -7355,7 +7355,7 @@
       <c r="G51" s="45"/>
       <c r="H51" s="308">
         <f>[1]CorporationTax!$D$34</f>
-        <v>45016</v>
+        <v>45260</v>
       </c>
       <c r="I51" s="309"/>
       <c r="J51" s="413"/>
@@ -9179,7 +9179,7 @@
     <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" s="234" t="str">
         <f>"Profit and Loss account for the year ended "&amp;TEXT(N2,"dd Mmm yyyy")</f>
-        <v>Profit and Loss account for the year ended 31 Mar 2023</v>
+        <v>Profit and Loss account for the year ended 30 Nov 2023</v>
       </c>
       <c r="B151" s="235"/>
       <c r="C151" s="235"/>
@@ -9286,7 +9286,7 @@
       <c r="E156" s="72"/>
       <c r="F156" s="418" t="str">
         <f>TEXT((YEARFRAC(J2,N2)*12),"0")&amp;" months to "&amp;TEXT(N2,"dd Mmm yyyy")&amp;"."</f>
-        <v>12 months to 31 Mar 2023.</v>
+        <v>12 months to 30 Nov 2023.</v>
       </c>
       <c r="G156" s="418"/>
       <c r="H156" s="418"/>
@@ -10518,7 +10518,7 @@
       <c r="E217" s="72"/>
       <c r="F217" s="238" t="str">
         <f>F156</f>
-        <v>12 months to 31 Mar 2023.</v>
+        <v>12 months to 30 Nov 2023.</v>
       </c>
       <c r="G217" s="239"/>
       <c r="H217" s="239"/>
@@ -10931,7 +10931,7 @@
     <row r="237" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A237" s="234" t="str">
         <f>"Balance sheet for the year ended "&amp;TEXT(N2,"dd Mmm yyyy")</f>
-        <v>Balance sheet for the year ended 31 Mar 2023</v>
+        <v>Balance sheet for the year ended 30 Nov 2023</v>
       </c>
       <c r="B237" s="235"/>
       <c r="C237" s="235"/>
@@ -12139,7 +12139,7 @@
     <row r="292" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A292" s="234" t="str">
         <f>"Balance sheet for the year ended "&amp;TEXT(N2,"dd Mmm yyyy")</f>
-        <v>Balance sheet for the year ended 31 Mar 2023</v>
+        <v>Balance sheet for the year ended 30 Nov 2023</v>
       </c>
       <c r="B292" s="235"/>
       <c r="C292" s="235"/>
@@ -15273,7 +15273,7 @@
       <c r="E470" s="72"/>
       <c r="F470" s="238" t="str">
         <f>F156</f>
-        <v>12 months to 31 Mar 2023.</v>
+        <v>12 months to 30 Nov 2023.</v>
       </c>
       <c r="G470" s="239"/>
       <c r="H470" s="239"/>
@@ -15744,7 +15744,7 @@
       <c r="E495" s="72"/>
       <c r="F495" s="238" t="str">
         <f>F156</f>
-        <v>12 months to 31 Mar 2023.</v>
+        <v>12 months to 30 Nov 2023.</v>
       </c>
       <c r="G495" s="239"/>
       <c r="H495" s="239"/>
@@ -16374,7 +16374,7 @@
       <c r="E527" s="72"/>
       <c r="F527" s="238" t="str">
         <f>F156</f>
-        <v>12 months to 31 Mar 2023.</v>
+        <v>12 months to 30 Nov 2023.</v>
       </c>
       <c r="G527" s="239"/>
       <c r="H527" s="239"/>
@@ -17488,7 +17488,7 @@
       <c r="E581" s="72"/>
       <c r="F581" s="238" t="str">
         <f>F156</f>
-        <v>12 months to 31 Mar 2023.</v>
+        <v>12 months to 30 Nov 2023.</v>
       </c>
       <c r="G581" s="238"/>
       <c r="H581" s="238"/>
@@ -17996,7 +17996,7 @@
     <row r="609" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A609" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B609" s="225"/>
       <c r="C609" s="283"/>
@@ -18363,7 +18363,7 @@
     <row r="626" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A626" s="265" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B626" s="305"/>
       <c r="C626" s="306"/>
@@ -18474,7 +18474,7 @@
     <row r="632" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A632" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B632" s="225"/>
       <c r="C632" s="283"/>
@@ -18757,7 +18757,7 @@
     <row r="645" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A645" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B645" s="225"/>
       <c r="C645" s="283"/>
@@ -18883,7 +18883,7 @@
     <row r="651" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A651" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B651" s="225"/>
       <c r="C651" s="283"/>
@@ -19201,7 +19201,7 @@
     <row r="668" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A668" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B668" s="225"/>
       <c r="C668" s="283"/>
@@ -19568,7 +19568,7 @@
     <row r="685" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A685" s="265" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B685" s="305"/>
       <c r="C685" s="306"/>
@@ -19679,7 +19679,7 @@
     <row r="691" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A691" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B691" s="225"/>
       <c r="C691" s="283"/>
@@ -19962,7 +19962,7 @@
     <row r="704" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A704" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B704" s="225"/>
       <c r="C704" s="283"/>
@@ -20088,7 +20088,7 @@
     <row r="710" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A710" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B710" s="225"/>
       <c r="C710" s="283"/>
@@ -20406,7 +20406,7 @@
     <row r="727" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A727" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B727" s="225"/>
       <c r="C727" s="283"/>
@@ -20773,7 +20773,7 @@
     <row r="744" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A744" s="265" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B744" s="305"/>
       <c r="C744" s="306"/>
@@ -20884,7 +20884,7 @@
     <row r="750" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A750" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B750" s="225"/>
       <c r="C750" s="283"/>
@@ -21167,7 +21167,7 @@
     <row r="763" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A763" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B763" s="225"/>
       <c r="C763" s="283"/>
@@ -21293,7 +21293,7 @@
     <row r="769" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A769" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B769" s="225"/>
       <c r="C769" s="283"/>
@@ -21611,7 +21611,7 @@
     <row r="786" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A786" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B786" s="225"/>
       <c r="C786" s="283"/>
@@ -21978,7 +21978,7 @@
     <row r="803" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A803" s="265" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B803" s="305"/>
       <c r="C803" s="306"/>
@@ -22089,7 +22089,7 @@
     <row r="809" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A809" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B809" s="225"/>
       <c r="C809" s="283"/>
@@ -22372,7 +22372,7 @@
     <row r="822" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A822" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B822" s="225"/>
       <c r="C822" s="283"/>
@@ -22498,7 +22498,7 @@
     <row r="828" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A828" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B828" s="225"/>
       <c r="C828" s="283"/>
@@ -22816,7 +22816,7 @@
     <row r="845" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A845" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B845" s="225"/>
       <c r="C845" s="283"/>
@@ -23183,7 +23183,7 @@
     <row r="862" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A862" s="265" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B862" s="305"/>
       <c r="C862" s="306"/>
@@ -23294,7 +23294,7 @@
     <row r="868" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A868" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B868" s="225"/>
       <c r="C868" s="283"/>
@@ -23577,7 +23577,7 @@
     <row r="881" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A881" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B881" s="225"/>
       <c r="C881" s="283"/>
@@ -23703,7 +23703,7 @@
     <row r="887" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A887" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B887" s="225"/>
       <c r="C887" s="283"/>
@@ -23981,7 +23981,7 @@
     <row r="902" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A902" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B902" s="225"/>
       <c r="C902" s="283"/>
@@ -24312,7 +24312,7 @@
     <row r="917" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A917" s="265" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B917" s="305"/>
       <c r="C917" s="306"/>
@@ -24423,7 +24423,7 @@
     <row r="923" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A923" s="224" t="str">
         <f>"At "&amp;TEXT(J2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 01 Apr 2022:</v>
+        <v>At 01 Dec 2022:</v>
       </c>
       <c r="B923" s="225"/>
       <c r="C923" s="283"/>
@@ -24688,7 +24688,7 @@
     <row r="935" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A935" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B935" s="225"/>
       <c r="C935" s="283"/>
@@ -24814,7 +24814,7 @@
     <row r="941" spans="1:17" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A941" s="224" t="str">
         <f>"At "&amp;TEXT(N2,"dd Mmm yyyy")&amp;":"</f>
-        <v>At 31 Mar 2023:</v>
+        <v>At 30 Nov 2023:</v>
       </c>
       <c r="B941" s="225"/>
       <c r="C941" s="283"/>
@@ -28709,7 +28709,7 @@
     <row r="1131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1131" s="224" t="str">
         <f>"Reserves at " &amp; TEXT(J2,"DD Mmm yyyy") &amp; ":"</f>
-        <v>Reserves at 01 Apr 2022:</v>
+        <v>Reserves at 01 Dec 2022:</v>
       </c>
       <c r="B1131" s="225"/>
       <c r="C1131" s="283"/>
@@ -28908,7 +28908,7 @@
     <row r="1140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1140" s="221" t="str">
         <f>"Retained profit at " &amp; TEXT(N2,"DD Mmm yyyy") &amp; ":"</f>
-        <v>Retained profit at 31 Mar 2023:</v>
+        <v>Retained profit at 30 Nov 2023:</v>
       </c>
       <c r="B1140" s="222"/>
       <c r="C1140" s="297"/>
@@ -30852,7 +30852,7 @@
     <row r="1237" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1237" s="266" t="str">
         <f>"Do your accounts start on " &amp; TEXT(J2,"dd Mmm yyyy") &amp; "?"</f>
-        <v>Do your accounts start on 01 Apr 2022?</v>
+        <v>Do your accounts start on 01 Dec 2022?</v>
       </c>
       <c r="B1237" s="266"/>
       <c r="C1237" s="266"/>
@@ -30884,7 +30884,7 @@
     <row r="1239" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1239" s="266" t="str">
         <f>"Do your accounts end on " &amp; TEXT(N2,"dd Mmm yyyy") &amp; "?"</f>
-        <v>Do your accounts end on 31 Mar 2023?</v>
+        <v>Do your accounts end on 30 Nov 2023?</v>
       </c>
       <c r="B1239" s="266"/>
       <c r="C1239" s="266"/>
@@ -30952,7 +30952,7 @@
       <c r="M1242" s="186"/>
       <c r="N1242" s="440">
         <f>J2</f>
-        <v>44652</v>
+        <v>44896</v>
       </c>
       <c r="O1242" s="441"/>
       <c r="P1242" s="26"/>
@@ -31016,7 +31016,7 @@
       <c r="M1245" s="107"/>
       <c r="N1245" s="442">
         <f>N2</f>
-        <v>45016</v>
+        <v>45260</v>
       </c>
       <c r="O1245" s="443"/>
       <c r="P1245" s="41"/>

</xml_diff>